<commit_message>
fixed computation of stats
</commit_message>
<xml_diff>
--- a/stats/results.xlsx
+++ b/stats/results.xlsx
@@ -458,39 +458,43 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Rewards</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1000</v>
+          <t>Steps On Failure</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>no failures!</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>no failures!</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>910.55</v>
+        <v>569.3</v>
       </c>
       <c r="E2" t="n">
-        <v>909.27</v>
+        <v>379.01</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Steps</t>
+          <t>Steps On Success</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>127.75</v>
+        <v>127.7549019607843</v>
       </c>
       <c r="C3" t="n">
-        <v>126.02</v>
+        <v>126.025</v>
       </c>
       <c r="D3" t="n">
-        <v>306.56</v>
+        <v>277.6</v>
       </c>
       <c r="E3" t="n">
-        <v>286.43</v>
+        <v>276.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
someone test this plz
</commit_message>
<xml_diff>
--- a/stats/results.xlsx
+++ b/stats/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,22 +436,52 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>L-1NANE</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>L3NAYE</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>L0NAYE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>L3NANE</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>L-1YANE</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>L1NAYE</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>L2NANE</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>L2NAYE</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>L3YANE</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>L2YANE</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>L2NANE</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>L3YANE</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>L3NANE</t>
         </is>
       </c>
     </row>
@@ -461,21 +491,39 @@
           <t>Steps On Failure</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>no failures!</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>no failures!</t>
-        </is>
+      <c r="B2" t="n">
+        <v>718.8</v>
+      </c>
+      <c r="C2" t="n">
+        <v>234.72</v>
       </c>
       <c r="D2" t="n">
-        <v>569.3</v>
+        <v>72.61</v>
       </c>
       <c r="E2" t="n">
         <v>379.01</v>
+      </c>
+      <c r="F2" t="n">
+        <v>870.4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>64.81999999999999</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>24</v>
+      </c>
+      <c r="J2" t="n">
+        <v>569.3</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -485,16 +533,34 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>127.7549019607843</v>
+        <v>413.66</v>
       </c>
       <c r="C3" t="n">
-        <v>126.025</v>
+        <v>281.85</v>
       </c>
       <c r="D3" t="n">
-        <v>277.6</v>
+        <v>81.98999999999999</v>
       </c>
       <c r="E3" t="n">
         <v>276.15</v>
+      </c>
+      <c r="F3" t="n">
+        <v>445.07</v>
+      </c>
+      <c r="G3" t="n">
+        <v>60.08</v>
+      </c>
+      <c r="H3" t="n">
+        <v>126.025</v>
+      </c>
+      <c r="I3" t="n">
+        <v>146.18</v>
+      </c>
+      <c r="J3" t="n">
+        <v>277.6</v>
+      </c>
+      <c r="K3" t="n">
+        <v>127.7549019607843</v>
       </c>
     </row>
   </sheetData>

</xml_diff>